<commit_message>
Improved peak detection algorithm, switched to using op505d part
</commit_message>
<xml_diff>
--- a/FastCalib.xlsx
+++ b/FastCalib.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Dist (cm)</t>
   </si>
@@ -34,6 +33,12 @@
   </si>
   <si>
     <t>log(FFT)</t>
+  </si>
+  <si>
+    <t>OP505D</t>
+  </si>
+  <si>
+    <t>NTE3037</t>
   </si>
 </sst>
 </file>
@@ -110,6 +115,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>NTE 3037 Calib Curve</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -339,11 +369,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="184137888"/>
-        <c:axId val="184131168"/>
+        <c:axId val="355054064"/>
+        <c:axId val="355054624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="184137888"/>
+        <c:axId val="355054064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -400,12 +430,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184131168"/>
+        <c:crossAx val="355054624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="184131168"/>
+        <c:axId val="355054624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -462,7 +492,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184137888"/>
+        <c:crossAx val="355054064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -526,6 +556,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>OP505D calib</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -565,6 +620,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FFT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -587,55 +653,87 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.11561132983377077"/>
+                  <c:y val="-0.34637357830271215"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$18</c:f>
+              <c:f>Sheet1!$D$3:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
+                <c:ptCount val="11"/>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
@@ -643,54 +741,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$18</c:f>
+              <c:f>Sheet1!$E$3:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>4.3213737826425782E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-0.14266750356873156</c:v>
-                </c:pt>
+                <c:ptCount val="11"/>
                 <c:pt idx="2">
-                  <c:v>-0.21467016498923297</c:v>
+                  <c:v>1.24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.29242982390206362</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.40893539297350079</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.42021640338318983</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.49485002168009401</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.55284196865778079</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.63827216398240705</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.6777807052660807</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.769551078621726</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.85387196432176193</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-0.88605664769316317</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-0.95860731484177497</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-1.0457574905606752</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -705,11 +785,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="184141248"/>
-        <c:axId val="184141808"/>
+        <c:axId val="355056864"/>
+        <c:axId val="357368304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="184141248"/>
+        <c:axId val="355056864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,12 +846,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184141808"/>
+        <c:crossAx val="357368304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="184141808"/>
+        <c:axId val="357368304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -828,7 +908,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184141248"/>
+        <c:crossAx val="355056864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1993,16 +2073,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2023,20 +2103,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>614362</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>385762</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2317,26 +2397,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>15</v>
       </c>
@@ -2348,7 +2443,7 @@
         <v>4.3213737826425782E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>18</v>
       </c>
@@ -2359,8 +2454,14 @@
         <f t="shared" si="0"/>
         <v>-0.14266750356873156</v>
       </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>1.24</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -2371,8 +2472,14 @@
         <f t="shared" si="0"/>
         <v>-0.21467016498923297</v>
       </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>22</v>
       </c>
@@ -2383,8 +2490,14 @@
         <f t="shared" si="0"/>
         <v>-0.29242982390206362</v>
       </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>0.45</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>25</v>
       </c>
@@ -2395,8 +2508,14 @@
         <f t="shared" si="0"/>
         <v>-0.40893539297350079</v>
       </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>0.28999999999999998</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>27</v>
       </c>
@@ -2407,8 +2526,14 @@
         <f t="shared" si="0"/>
         <v>-0.42021640338318983</v>
       </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <v>0.21</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>30</v>
       </c>
@@ -2419,8 +2544,14 @@
         <f t="shared" si="0"/>
         <v>-0.49485002168009401</v>
       </c>
+      <c r="D10">
+        <v>35</v>
+      </c>
+      <c r="E10">
+        <v>0.16</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>32</v>
       </c>
@@ -2431,8 +2562,14 @@
         <f t="shared" si="0"/>
         <v>-0.55284196865778079</v>
       </c>
+      <c r="D11">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <v>0.13</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>35</v>
       </c>
@@ -2443,8 +2580,14 @@
         <f t="shared" si="0"/>
         <v>-0.63827216398240705</v>
       </c>
+      <c r="D12">
+        <v>45</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>37</v>
       </c>
@@ -2455,8 +2598,14 @@
         <f t="shared" si="0"/>
         <v>-0.6777807052660807</v>
       </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>0.08</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>40</v>
       </c>
@@ -2468,7 +2617,7 @@
         <v>-0.769551078621726</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>42</v>
       </c>
@@ -2480,7 +2629,7 @@
         <v>-0.85387196432176193</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
minor pcb and BOM adjustments
</commit_message>
<xml_diff>
--- a/FastCalib.xlsx
+++ b/FastCalib.xlsx
@@ -369,11 +369,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="355054064"/>
-        <c:axId val="355054624"/>
+        <c:axId val="153423344"/>
+        <c:axId val="153423904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="355054064"/>
+        <c:axId val="153423344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -430,12 +430,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="355054624"/>
+        <c:crossAx val="153423904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="355054624"/>
+        <c:axId val="153423904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +492,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="355054064"/>
+        <c:crossAx val="153423344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -785,11 +785,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="355056864"/>
-        <c:axId val="357368304"/>
+        <c:axId val="153426144"/>
+        <c:axId val="153426704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="355056864"/>
+        <c:axId val="153426144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,12 +846,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357368304"/>
+        <c:crossAx val="153426704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="357368304"/>
+        <c:axId val="153426704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -908,7 +908,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="355056864"/>
+        <c:crossAx val="153426144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2399,7 +2399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>

</xml_diff>